<commit_message>
refactoring + UML update !
</commit_message>
<xml_diff>
--- a/TODO_TEAM.xlsx
+++ b/TODO_TEAM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="21">
   <si>
     <t>Description:</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Bordure qui clignote</t>
+  </si>
+  <si>
+    <t>IA ennemi?</t>
+  </si>
+  <si>
+    <t>Initialiser la liste de Filtres (avec une Factory peut etre) (Gesture)</t>
+  </si>
+  <si>
+    <t>Mettre a jour le diagramme de classe en cas de mofication du CODE !!!!!!</t>
   </si>
 </sst>
 </file>
@@ -612,8 +621,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:D22" totalsRowShown="0">
-  <autoFilter ref="A1:D22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:D23" totalsRowShown="0">
+  <autoFilter ref="A1:D23"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Description:"/>
     <tableColumn id="4" name="Assigné à:"/>
@@ -911,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -951,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -965,10 +974,10 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -979,43 +988,52 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -1023,10 +1041,10 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -1034,10 +1052,10 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -1045,10 +1063,10 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
@@ -1056,10 +1074,10 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1067,10 +1085,10 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1078,10 +1096,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -1089,10 +1107,10 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -1100,10 +1118,10 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1111,10 +1129,10 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -1122,10 +1140,10 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -1133,10 +1151,10 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
@@ -1144,10 +1162,10 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1155,10 +1173,10 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>15</v>
       </c>
@@ -1166,10 +1184,10 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -1177,10 +1195,21 @@
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1188,30 +1217,24 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Variables!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C22</xm:sqref>
+          <xm:sqref>C2:C23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Variables!$C:$C</xm:f>
           </x14:formula1>
-          <xm:sqref>C23:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Variables!$C:$C</xm:f>
-          </x14:formula1>
-          <xm:sqref>D1:D22</xm:sqref>
+          <xm:sqref>C24:C1048576 D1:D23</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Variables!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B22</xm:sqref>
+          <xm:sqref>B2:B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
maj rotation + gesture + debut weapon avoid player
</commit_message>
<xml_diff>
--- a/TODO_TEAM.xlsx
+++ b/TODO_TEAM.xlsx
@@ -11,12 +11,11 @@
     <sheet name="Variables" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
   <si>
     <t>Description:</t>
   </si>
@@ -99,7 +98,7 @@
     <t>Moyen</t>
   </si>
   <si>
-    <t xml:space="preserve">TO BE TEST </t>
+    <t>Corrigé -&gt; to be test</t>
   </si>
 </sst>
 </file>
@@ -140,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -453,7 +453,7 @@
     <col min="14" max="1025" width="11.375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" outlineLevel="1">
+    <row r="2" spans="1:4" outlineLevel="1">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -481,7 +481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" outlineLevel="1">
+    <row r="3" spans="1:4" outlineLevel="1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -495,7 +495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" outlineLevel="1">
+    <row r="4" spans="1:4" outlineLevel="1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -509,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" outlineLevel="1">
+    <row r="5" spans="1:4" outlineLevel="1">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -523,7 +523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" outlineLevel="1">
+    <row r="6" spans="1:4" outlineLevel="1">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -537,7 +537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" outlineLevel="1">
+    <row r="7" spans="1:4" outlineLevel="1">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -551,8 +551,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" outlineLevel="1">
-      <c r="A8" t="s">
+    <row r="8" spans="1:4" outlineLevel="1">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
@@ -565,7 +565,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" outlineLevel="1">
+    <row r="9" spans="1:4" outlineLevel="1">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -579,7 +579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" outlineLevel="1">
+    <row r="10" spans="1:4" outlineLevel="1">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -593,7 +593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" outlineLevel="1">
+    <row r="11" spans="1:4" outlineLevel="1">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -604,13 +604,10 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" outlineLevel="1">
+    <row r="12" spans="1:4" outlineLevel="1">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -621,10 +618,10 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" outlineLevel="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" outlineLevel="1">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -638,7 +635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" outlineLevel="1">
+    <row r="14" spans="1:4" outlineLevel="1">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -649,7 +646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" outlineLevel="1">
+    <row r="15" spans="1:4" outlineLevel="1">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -660,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" outlineLevel="1">
+    <row r="16" spans="1:4" outlineLevel="1">
       <c r="B16" t="s">
         <v>15</v>
       </c>

</xml_diff>